<commit_message>
Added results part I and model selection
</commit_message>
<xml_diff>
--- a/modeling/results/feature_imp_attr.xlsx
+++ b/modeling/results/feature_imp_attr.xlsx
@@ -22,582 +22,597 @@
     <t>Importance</t>
   </si>
   <si>
+    <t>Quant</t>
+  </si>
+  <si>
+    <t>CRIME DA LEI DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos LIBERDADE PROVISÓRIA</t>
+  </si>
+  <si>
+    <t>Relator_MARCO AURÉLIO</t>
+  </si>
+  <si>
     <t>diff_datas</t>
   </si>
   <si>
-    <t>Quant</t>
+    <t>origem_SP - SÃO PAULO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO PREVENTIVA</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A PESSOA</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE</t>
+  </si>
+  <si>
+    <t>assuntos REVOGAÇÃO</t>
+  </si>
+  <si>
+    <t>Relator_LUIZ FUX</t>
+  </si>
+  <si>
+    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
+  </si>
+  <si>
+    <t>origem_AL - ALAGOAS</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
+  </si>
+  <si>
+    <t>Relator_ROSA WEBER</t>
+  </si>
+  <si>
+    <t>Relator_ROBERTO BARROSO</t>
+  </si>
+  <si>
+    <t>Relator_RICARDO LEWANDOWSKI</t>
+  </si>
+  <si>
+    <t>Relator_DIAS TOFFOLI</t>
+  </si>
+  <si>
+    <t>assuntos LIVRAMENTO CONDICIONAL</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
+  </si>
+  <si>
+    <t>CRIME DA LEI DE ARMAS</t>
+  </si>
+  <si>
+    <t>Relator_CÁRMEN LÚCIA</t>
   </si>
   <si>
     <t>assuntos FURTO QUALIFICADO</t>
   </si>
   <si>
-    <t>CRIME CONTRA A PESSOA</t>
+    <t>assuntos PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL PENAL</t>
+  </si>
+  <si>
+    <t>assuntos INVESTIGAÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>assuntos TRANCAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos PRINCÍPIO DA INSIGNIFICÂNCIA</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL</t>
   </si>
   <si>
     <t>origem_PB - PARAÍBA</t>
   </si>
   <si>
-    <t>Relator_MARCO AURÉLIO</t>
+    <t>origem_MG - MINAS GERAIS</t>
+  </si>
+  <si>
+    <t>origem_RO - RONDÔNIA</t>
+  </si>
+  <si>
+    <t>origem_RR - RORAIMA</t>
+  </si>
+  <si>
+    <t>origem_RS - RIO GRANDE DO SUL</t>
+  </si>
+  <si>
+    <t>origem_PI - PIAUÍ</t>
   </si>
   <si>
     <t>origem_PE - PERNAMBUCO</t>
   </si>
   <si>
-    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
+    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>origem_RJ - RIO DE JANEIRO</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
+  </si>
+  <si>
+    <t>assuntos FIANÇA</t>
+  </si>
+  <si>
+    <t>origem_TO - TOCANTINS</t>
+  </si>
+  <si>
+    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
+  </si>
+  <si>
+    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
+  </si>
+  <si>
+    <t>assuntos REGRESSÃO DE REGIME</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
+  </si>
+  <si>
+    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES HEDIONDOS</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
+  </si>
+  <si>
+    <t>assuntos EMPRESAS</t>
+  </si>
+  <si>
+    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos TRATAMENTO AMBULATORIAL</t>
+  </si>
+  <si>
+    <t>assuntos PRESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos IMPEDIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos MANDATO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
+  </si>
+  <si>
+    <t>assuntos PROGRESSÃO DE REGIME</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A VIDA</t>
+  </si>
+  <si>
+    <t>assuntos REGIME INICIAL</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
+  </si>
+  <si>
+    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos QUADRILHA OU BANDO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL</t>
+  </si>
+  <si>
+    <t>assuntos ABOLITIO CRIMINIS</t>
+  </si>
+  <si>
+    <t>Relator_CEZAR PELUSO</t>
+  </si>
+  <si>
+    <t>assuntos ESTRANGEIRO</t>
+  </si>
+  <si>
+    <t>origem_GO - GOIÁS</t>
+  </si>
+  <si>
+    <t>origem_AC - ACRE</t>
+  </si>
+  <si>
+    <t>origem_AM - AMAZONAS</t>
+  </si>
+  <si>
+    <t>origem_AP - AMAPÁ</t>
+  </si>
+  <si>
+    <t>origem_BA - BAHIA</t>
+  </si>
+  <si>
+    <t>origem_CE - CEARÁ</t>
+  </si>
+  <si>
+    <t>origem_DF - DISTRITO FEDERAL</t>
+  </si>
+  <si>
+    <t>origem_ES - ESPÍRITO SANTO</t>
+  </si>
+  <si>
+    <t>origem_MA - MARANHÃO</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>origem_MS - MATO GROSSO DO SUL</t>
+  </si>
+  <si>
+    <t>origem_MT - MATO GROSSO</t>
+  </si>
+  <si>
+    <t>origem_PA - PARÁ</t>
+  </si>
+  <si>
+    <t>origem_PR - PARANÁ</t>
+  </si>
+  <si>
+    <t>origem_RN - RIO GRANDE DO NORTE</t>
+  </si>
+  <si>
+    <t>origem_SC - SANTA CATARINA</t>
+  </si>
+  <si>
+    <t>origem_SE - SERGIPE</t>
+  </si>
+  <si>
+    <t>Relator_TEORI ZAVASCKI</t>
+  </si>
+  <si>
+    <t>Relator_OCTAVIO GALLOTTI</t>
+  </si>
+  <si>
+    <t>Relator_MOREIRA ALVES</t>
+  </si>
+  <si>
+    <t>Relator_JOAQUIM BARBOSA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
+  </si>
+  <si>
+    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
+  </si>
+  <si>
+    <t>Relator_ALEXANDRE DE MORAES</t>
+  </si>
+  <si>
+    <t>Relator_AYRES BRITTO</t>
+  </si>
+  <si>
+    <t>Relator_CARLOS VELLOSO</t>
+  </si>
+  <si>
+    <t>Relator_CELSO DE MELLO</t>
+  </si>
+  <si>
+    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
+  </si>
+  <si>
+    <t>Relator_EDSON FACHIN</t>
+  </si>
+  <si>
+    <t>Relator_ELLEN GRACIE</t>
+  </si>
+  <si>
+    <t>Relator_EROS GRAU</t>
+  </si>
+  <si>
+    <t>Relator_FRANCISCO REZEK</t>
+  </si>
+  <si>
+    <t>Relator_GILMAR MENDES</t>
+  </si>
+  <si>
+    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
+  </si>
+  <si>
+    <t>Relator_ILMAR GALVÃO</t>
+  </si>
+  <si>
+    <t>assuntos PREFEITO</t>
+  </si>
+  <si>
+    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO EM FLAGRANTE</t>
+  </si>
+  <si>
+    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE OU ANULAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
+  </si>
+  <si>
+    <t>assuntos PROVAS</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO CIVIL</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO (ART. 157)</t>
+  </si>
+  <si>
+    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
+  </si>
+  <si>
+    <t>assuntos RECEPTAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
+  </si>
+  <si>
+    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos ELEIÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos JURISDIÇÃO E COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
+  </si>
+  <si>
+    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos FURTO</t>
+  </si>
+  <si>
+    <t>assuntos PARTE GERAL</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>DESCONHECIDO</t>
+  </si>
+  <si>
+    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>assuntos AFASTAMENTO DO CARGO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos CORRUPÇÃO PASSIVA</t>
+  </si>
+  <si>
+    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos EXTRADIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>assuntos RECURSO</t>
+  </si>
+  <si>
+    <t>assuntos INDULTO</t>
+  </si>
+  <si>
+    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO</t>
+  </si>
+  <si>
+    <t>assuntos HOMICÍDIO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DO MP</t>
+  </si>
+  <si>
+    <t>assuntos TRIBUNAL DE CONTAS</t>
+  </si>
+  <si>
+    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A PAZ PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES MILITARES</t>
+  </si>
+  <si>
+    <t>assuntos FATOS JURÍDICOS</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos ASSUNTOS DIVERSOS</t>
+  </si>
+  <si>
+    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos TIPICIDADE</t>
+  </si>
+  <si>
+    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos PROVA ILÍCITA</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
+  </si>
+  <si>
+    <t>assuntos SUSPEIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos FURTO (ART. 155)</t>
+  </si>
+  <si>
+    <t>assuntos Desconhecido</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO MAJORADO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ELEITORAL</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
+  </si>
+  <si>
+    <t>assuntos MEDIDAS DE SEGURANÇA</t>
+  </si>
+  <si>
+    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ELEITORAL E PROCESSO ELEITORAL</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS</t>
+  </si>
+  <si>
+    <t>assuntos DENEGAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO TEMPORÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
+  </si>
+  <si>
+    <t>assuntos SUSPENSÃO</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL MILITAR</t>
   </si>
   <si>
     <t>assuntos INDEFERIMENTO</t>
   </si>
   <si>
-    <t>assuntos TRANCAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos INVESTIGAÇÃO PENAL</t>
+    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
+  </si>
+  <si>
+    <t>assuntos AGENTES POLÍTICOS</t>
+  </si>
+  <si>
+    <t>assuntos ESTELIONATO MAJORADO</t>
   </si>
   <si>
     <t>assuntos CERCEAMENTO DE DEFESA</t>
   </si>
   <si>
-    <t>Relator_CELSO DE MELLO</t>
-  </si>
-  <si>
-    <t>Relator_CÁRMEN LÚCIA</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL MILITAR</t>
+    <t>assuntos APLICAÇÃO DA PENA</t>
   </si>
   <si>
     <t>assuntos DENÚNCIA/QUEIXA</t>
   </si>
   <si>
-    <t>assuntos SUSPENSÃO</t>
-  </si>
-  <si>
-    <t>Relator_EDSON FACHIN</t>
-  </si>
-  <si>
-    <t>Relator_GILMAR MENDES</t>
-  </si>
-  <si>
-    <t>Relator_ILMAR GALVÃO</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
-  </si>
-  <si>
-    <t>Relator_OCTAVIO GALLOTTI</t>
-  </si>
-  <si>
-    <t>Relator_RICARDO LEWANDOWSKI</t>
-  </si>
-  <si>
-    <t>Relator_CARLOS VELLOSO</t>
+    <t>assuntos ATO INFRACIONAL</t>
+  </si>
+  <si>
+    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
   </si>
   <si>
     <t>assuntos DESCLASSIFICAÇÃO</t>
   </si>
   <si>
-    <t>Relator_AYRES BRITTO</t>
-  </si>
-  <si>
-    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
-  </si>
-  <si>
-    <t>assuntos LIBERDADE PROVISÓRIA</t>
-  </si>
-  <si>
-    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos QUADRILHA OU BANDO</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
-  </si>
-  <si>
-    <t>assuntos LIVRAMENTO CONDICIONAL</t>
-  </si>
-  <si>
-    <t>CRIME DA LEI DE ARMAS</t>
-  </si>
-  <si>
-    <t>assuntos PROGRESSÃO DE REGIME</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
-  </si>
-  <si>
-    <t>assuntos PRINCÍPIO DA INSIGNIFICÂNCIA</t>
-  </si>
-  <si>
-    <t>assuntos FURTO (ART. 155)</t>
-  </si>
-  <si>
-    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
+    <t>assuntos CONTRA A VIDA</t>
   </si>
   <si>
     <t>assuntos LICITAÇÕES</t>
   </si>
   <si>
-    <t>assuntos PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
-  </si>
-  <si>
-    <t>assuntos NULIDADE</t>
-  </si>
-  <si>
-    <t>Relator_ROBERTO BARROSO</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
-  </si>
-  <si>
-    <t>origem_RO - RONDÔNIA</t>
-  </si>
-  <si>
-    <t>origem_MS - MATO GROSSO DO SUL</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>assuntos INDULTO</t>
-  </si>
-  <si>
-    <t>assuntos FIANÇA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>origem_PA - PARÁ</t>
-  </si>
-  <si>
-    <t>origem_PI - PIAUÍ</t>
-  </si>
-  <si>
-    <t>origem_PR - PARANÁ</t>
-  </si>
-  <si>
-    <t>origem_DF - DISTRITO FEDERAL</t>
-  </si>
-  <si>
-    <t>origem_CE - CEARÁ</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
-  </si>
-  <si>
-    <t>assuntos PROVAS</t>
-  </si>
-  <si>
-    <t>origem_RR - RORAIMA</t>
-  </si>
-  <si>
-    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
-  </si>
-  <si>
-    <t>origem_SP - SÃO PAULO</t>
-  </si>
-  <si>
-    <t>origem_AP - AMAPÁ</t>
-  </si>
-  <si>
-    <t>origem_AL - ALAGOAS</t>
-  </si>
-  <si>
-    <t>origem_AC - ACRE</t>
-  </si>
-  <si>
-    <t>origem_TO - TOCANTINS</t>
-  </si>
-  <si>
-    <t>Relator_TEORI ZAVASCKI</t>
-  </si>
-  <si>
-    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
-  </si>
-  <si>
-    <t>assuntos PRESCRIÇÃO</t>
-  </si>
-  <si>
-    <t>origem_RN - RIO GRANDE DO NORTE</t>
-  </si>
-  <si>
-    <t>assuntos MANDATO</t>
-  </si>
-  <si>
-    <t>assuntos TRATAMENTO AMBULATORIAL</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO PREVENTIVA</t>
-  </si>
-  <si>
-    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>Relator_ROSA WEBER</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
-  </si>
-  <si>
-    <t>origem_RS - RIO GRANDE DO SUL</t>
-  </si>
-  <si>
-    <t>assuntos REVOGAÇÃO</t>
-  </si>
-  <si>
-    <t>origem_SC - SANTA CATARINA</t>
-  </si>
-  <si>
-    <t>assuntos REGIME INICIAL</t>
-  </si>
-  <si>
-    <t>origem_SE - SERGIPE</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos IMPEDIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES HEDIONDOS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>Relator_MOREIRA ALVES</t>
-  </si>
-  <si>
-    <t>Relator_LUIZ FUX</t>
-  </si>
-  <si>
-    <t>Relator_JOAQUIM BARBOSA</t>
-  </si>
-  <si>
-    <t>origem_AM - AMAZONAS</t>
-  </si>
-  <si>
-    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
-  </si>
-  <si>
-    <t>Relator_FRANCISCO REZEK</t>
-  </si>
-  <si>
-    <t>Relator_EROS GRAU</t>
-  </si>
-  <si>
-    <t>Relator_ELLEN GRACIE</t>
-  </si>
-  <si>
-    <t>origem_BA - BAHIA</t>
-  </si>
-  <si>
-    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>Relator_DIAS TOFFOLI</t>
-  </si>
-  <si>
-    <t>origem_ES - ESPÍRITO SANTO</t>
-  </si>
-  <si>
-    <t>Relator_CEZAR PELUSO</t>
-  </si>
-  <si>
-    <t>origem_GO - GOIÁS</t>
-  </si>
-  <si>
-    <t>origem_MA - MARANHÃO</t>
-  </si>
-  <si>
-    <t>origem_MG - MINAS GERAIS</t>
-  </si>
-  <si>
-    <t>origem_MT - MATO GROSSO</t>
-  </si>
-  <si>
-    <t>Relator_ALEXANDRE DE MORAES</t>
-  </si>
-  <si>
-    <t>origem_RJ - RIO DE JANEIRO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos ESTRANGEIRO</t>
-  </si>
-  <si>
-    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos ABOLITIO CRIMINIS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
-  </si>
-  <si>
-    <t>assuntos EMPRESAS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ELEITORAL</t>
-  </si>
-  <si>
-    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO EM FLAGRANTE</t>
-  </si>
-  <si>
-    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos NULIDADE OU ANULAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos EXECUÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO CIVIL</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO (ART. 157)</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DO MP</t>
-  </si>
-  <si>
-    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
-  </si>
-  <si>
-    <t>assuntos RECEPTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos ELEIÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos JURISDIÇÃO E COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos HOMICÍDIO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos PARTE GERAL</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO</t>
-  </si>
-  <si>
-    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
-  </si>
-  <si>
-    <t>CRIME DA LEI DE DROGAS</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>DESCONHECIDO</t>
-  </si>
-  <si>
-    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>assuntos AFASTAMENTO DO CARGO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos CORRUPÇÃO PASSIVA</t>
-  </si>
-  <si>
-    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos EXTRADIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
-  </si>
-  <si>
-    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>assuntos RECURSO</t>
-  </si>
-  <si>
-    <t>assuntos FURTO</t>
-  </si>
-  <si>
-    <t>assuntos DENEGAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A VIDA</t>
-  </si>
-  <si>
-    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
-  </si>
-  <si>
-    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos TIPICIDADE</t>
-  </si>
-  <si>
-    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos PROVA ILÍCITA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
-  </si>
-  <si>
-    <t>assuntos SUSPEIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos Desconhecido</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
-  </si>
-  <si>
-    <t>assuntos MEDIDAS DE SEGURANÇA</t>
-  </si>
-  <si>
-    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
-  </si>
-  <si>
-    <t>assuntos TRIBUNAL DE CONTAS</t>
-  </si>
-  <si>
-    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>assuntos PREFEITO</t>
-  </si>
-  <si>
-    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
-  </si>
-  <si>
-    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos REGRESSÃO DE REGIME</t>
-  </si>
-  <si>
-    <t>assuntos ASSUNTOS DIVERSOS</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos FATOS JURÍDICOS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES MILITARES</t>
-  </si>
-  <si>
-    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
-  </si>
-  <si>
-    <t>assuntos AGENTES POLÍTICOS</t>
-  </si>
-  <si>
-    <t>assuntos ESTELIONATO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL PENAL</t>
-  </si>
-  <si>
-    <t>assuntos APLICAÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos ATO INFRACIONAL</t>
-  </si>
-  <si>
-    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A VIDA</t>
-  </si>
-  <si>
     <t>assuntos INSERÇÃO DE DADOS FALSOS EM SISTEMA DE INFORMAÇÕES</t>
   </si>
   <si>
@@ -608,21 +623,6 @@
   </si>
   <si>
     <t>assuntos RECUPERAÇÃO JUDICIAL E FALÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO TEMPORÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS</t>
-  </si>
-  <si>
-    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ELEITORAL E PROCESSO ELEITORAL</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A PAZ PÚBLICA</t>
   </si>
   <si>
     <t>assuntos FURTO DE COISA COMUM</t>
@@ -1002,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.02</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.02</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.02</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2">

</xml_diff>

<commit_message>
Adjustments on modelling and model seelction
</commit_message>
<xml_diff>
--- a/modeling/results/feature_imp_attr.xlsx
+++ b/modeling/results/feature_imp_attr.xlsx
@@ -22,607 +22,607 @@
     <t>Importance</t>
   </si>
   <si>
+    <t>diff_datas</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO PREVENTIVA</t>
+  </si>
+  <si>
+    <t>Relator_MARCO AURÉLIO</t>
+  </si>
+  <si>
+    <t>origem_SP - SÃO PAULO</t>
+  </si>
+  <si>
+    <t>assuntos REVOGAÇÃO</t>
+  </si>
+  <si>
+    <t>Relator_JOAQUIM BARBOSA</t>
+  </si>
+  <si>
+    <t>assuntos LIBERDADE PROVISÓRIA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A VIDA</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
+  </si>
+  <si>
+    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos PROGRESSÃO DE REGIME</t>
+  </si>
+  <si>
+    <t>assuntos LIVRAMENTO CONDICIONAL</t>
+  </si>
+  <si>
+    <t>assuntos REGIME INICIAL</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
+  </si>
+  <si>
+    <t>assuntos PREFEITO</t>
+  </si>
+  <si>
+    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ELEITORAL</t>
+  </si>
+  <si>
+    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
+  </si>
+  <si>
+    <t>assuntos PROVA ILÍCITA</t>
+  </si>
+  <si>
+    <t>assuntos TIPICIDADE</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO TEMPORÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos ATOS PROCESSUAIS</t>
+  </si>
+  <si>
+    <t>assuntos LICITAÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos DESCLASSIFICAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
+  </si>
+  <si>
+    <t>Relator_AYRES BRITTO</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE</t>
+  </si>
+  <si>
+    <t>assuntos CERCEAMENTO DE DEFESA</t>
+  </si>
+  <si>
+    <t>origem_SC - SANTA CATARINA</t>
+  </si>
+  <si>
+    <t>origem_RR - RORAIMA</t>
+  </si>
+  <si>
+    <t>origem_RO - RONDÔNIA</t>
+  </si>
+  <si>
+    <t>origem_RN - RIO GRANDE DO NORTE</t>
+  </si>
+  <si>
+    <t>origem_PE - PERNAMBUCO</t>
+  </si>
+  <si>
+    <t>origem_PB - PARAÍBA</t>
+  </si>
+  <si>
+    <t>origem_MS - MATO GROSSO DO SUL</t>
+  </si>
+  <si>
+    <t>origem_ES - ESPÍRITO SANTO</t>
+  </si>
+  <si>
+    <t>origem_CE - CEARÁ</t>
+  </si>
+  <si>
+    <t>origem_AP - AMAPÁ</t>
+  </si>
+  <si>
+    <t>origem_AC - ACRE</t>
+  </si>
+  <si>
+    <t>Relator_TEORI ZAVASCKI</t>
+  </si>
+  <si>
+    <t>Relator_ROBERTO BARROSO</t>
+  </si>
+  <si>
+    <t>Relator_RICARDO LEWANDOWSKI</t>
+  </si>
+  <si>
+    <t>Relator_OCTAVIO GALLOTTI</t>
+  </si>
+  <si>
+    <t>Relator_MOREIRA ALVES</t>
+  </si>
+  <si>
+    <t>Relator_LUIZ FUX</t>
+  </si>
+  <si>
+    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
+  </si>
+  <si>
+    <t>Relator_DIAS TOFFOLI</t>
+  </si>
+  <si>
+    <t>Relator_CÁRMEN LÚCIA</t>
+  </si>
+  <si>
+    <t>Relator_CEZAR PELUSO</t>
+  </si>
+  <si>
+    <t>Relator_CELSO DE MELLO</t>
+  </si>
+  <si>
+    <t>Relator_CARLOS VELLOSO</t>
+  </si>
+  <si>
+    <t>assuntos INVESTIGAÇÃO PENAL</t>
+  </si>
+  <si>
     <t>Quant</t>
   </si>
   <si>
+    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>CRIME DA LEI DE ARMAS</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A PESSOA</t>
+  </si>
+  <si>
+    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
+  </si>
+  <si>
+    <t>assuntos INDULTO</t>
+  </si>
+  <si>
+    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos FIANÇA</t>
+  </si>
+  <si>
+    <t>Relator_ALEXANDRE DE MORAES</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
+  </si>
+  <si>
+    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO</t>
+  </si>
+  <si>
+    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
+  </si>
+  <si>
+    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>Relator_EDSON FACHIN</t>
+  </si>
+  <si>
+    <t>Relator_ELLEN GRACIE</t>
+  </si>
+  <si>
+    <t>Relator_EROS GRAU</t>
+  </si>
+  <si>
+    <t>assuntos RECURSO</t>
+  </si>
+  <si>
+    <t>assuntos ESTRANGEIRO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>Relator_GILMAR MENDES</t>
+  </si>
+  <si>
+    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos ABOLITIO CRIMINIS</t>
+  </si>
+  <si>
+    <t>assuntos PARTE GERAL</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO EM FLAGRANTE</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES HEDIONDOS</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
+  </si>
+  <si>
+    <t>assuntos TRATAMENTO AMBULATORIAL</t>
+  </si>
+  <si>
+    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos PRESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>Relator_FRANCISCO REZEK</t>
+  </si>
+  <si>
+    <t>assuntos EXTRADIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>Relator_ILMAR GALVÃO</t>
+  </si>
+  <si>
+    <t>origem_TO - TOCANTINS</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>origem_SE - SERGIPE</t>
+  </si>
+  <si>
+    <t>origem_RS - RIO GRANDE DO SUL</t>
+  </si>
+  <si>
     <t>CRIME DA LEI DE DROGAS</t>
   </si>
   <si>
-    <t>assuntos LIBERDADE PROVISÓRIA</t>
-  </si>
-  <si>
-    <t>Relator_MARCO AURÉLIO</t>
-  </si>
-  <si>
-    <t>diff_datas</t>
-  </si>
-  <si>
-    <t>origem_SP - SÃO PAULO</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO PREVENTIVA</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A PESSOA</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos NULIDADE</t>
-  </si>
-  <si>
-    <t>assuntos REVOGAÇÃO</t>
-  </si>
-  <si>
-    <t>Relator_LUIZ FUX</t>
-  </si>
-  <si>
-    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
+    <t>origem_RJ - RIO DE JANEIRO</t>
+  </si>
+  <si>
+    <t>origem_PR - PARANÁ</t>
+  </si>
+  <si>
+    <t>origem_PI - PIAUÍ</t>
+  </si>
+  <si>
+    <t>origem_PA - PARÁ</t>
+  </si>
+  <si>
+    <t>origem_MT - MATO GROSSO</t>
+  </si>
+  <si>
+    <t>DESCONHECIDO</t>
+  </si>
+  <si>
+    <t>origem_MG - MINAS GERAIS</t>
+  </si>
+  <si>
+    <t>origem_MA - MARANHÃO</t>
+  </si>
+  <si>
+    <t>origem_GO - GOIÁS</t>
+  </si>
+  <si>
+    <t>origem_DF - DISTRITO FEDERAL</t>
+  </si>
+  <si>
+    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>origem_BA - BAHIA</t>
+  </si>
+  <si>
+    <t>origem_AM - AMAZONAS</t>
   </si>
   <si>
     <t>origem_AL - ALAGOAS</t>
   </si>
   <si>
-    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
+    <t>assuntos AFASTAMENTO DO CARGO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
   </si>
   <si>
     <t>Relator_ROSA WEBER</t>
   </si>
   <si>
-    <t>Relator_ROBERTO BARROSO</t>
-  </si>
-  <si>
-    <t>Relator_RICARDO LEWANDOWSKI</t>
-  </si>
-  <si>
-    <t>Relator_DIAS TOFFOLI</t>
-  </si>
-  <si>
-    <t>assuntos LIVRAMENTO CONDICIONAL</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
-  </si>
-  <si>
-    <t>CRIME DA LEI DE ARMAS</t>
-  </si>
-  <si>
-    <t>Relator_CÁRMEN LÚCIA</t>
+    <t>assuntos CRIMES ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos CORRUPÇÃO PASSIVA</t>
+  </si>
+  <si>
+    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos MANDATO</t>
+  </si>
+  <si>
+    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
   </si>
   <si>
     <t>assuntos FURTO QUALIFICADO</t>
   </si>
   <si>
+    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
+  </si>
+  <si>
+    <t>assuntos INSERÇÃO DE DADOS FALSOS EM SISTEMA DE INFORMAÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos JURISDIÇÃO E COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos RECEPTAÇÃO QUALIFICADA</t>
+  </si>
+  <si>
+    <t>assuntos RECUPERAÇÃO JUDICIAL E FALÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos ELEIÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ELEITORAL E PROCESSO ELEITORAL</t>
+  </si>
+  <si>
     <t>assuntos PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
   </si>
   <si>
+    <t>assuntos CRIMES CONTRA A PAZ PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES MILITARES</t>
+  </si>
+  <si>
+    <t>assuntos FATOS JURÍDICOS</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos ASSUNTOS DIVERSOS</t>
+  </si>
+  <si>
+    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos HOMICÍDIO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA A VIDA</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE OU ANULAÇÃO</t>
+  </si>
+  <si>
     <t>assuntos DIREITO PROCESSUAL PENAL</t>
   </si>
   <si>
-    <t>assuntos INVESTIGAÇÃO PENAL</t>
+    <t>assuntos SUSPENSÃO</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos INDEFERIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
+  </si>
+  <si>
+    <t>assuntos AGENTES POLÍTICOS</t>
+  </si>
+  <si>
+    <t>assuntos ESTELIONATO MAJORADO</t>
+  </si>
+  <si>
+    <t>assuntos DENEGAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos FURTO</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DO MP</t>
   </si>
   <si>
     <t>assuntos TRANCAMENTO</t>
   </si>
   <si>
+    <t>assuntos APLICAÇÃO DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos DENÚNCIA/QUEIXA</t>
+  </si>
+  <si>
+    <t>assuntos ATO INFRACIONAL</t>
+  </si>
+  <si>
+    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos IMPEDIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos REGRESSÃO DE REGIME</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO CIVIL</t>
+  </si>
+  <si>
+    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
+  </si>
+  <si>
+    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos EMPRESAS</t>
+  </si>
+  <si>
+    <t>assuntos PROVAS</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
+  </si>
+  <si>
+    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos QUADRILHA OU BANDO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO (ART. 157)</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos TRIBUNAL DE CONTAS</t>
+  </si>
+  <si>
+    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
+  </si>
+  <si>
+    <t>assuntos MEDIDAS DE SEGURANÇA</t>
+  </si>
+  <si>
+    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
+  </si>
+  <si>
+    <t>assuntos RECEPTAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
+  </si>
+  <si>
+    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO MAJORADO</t>
+  </si>
+  <si>
+    <t>assuntos Desconhecido</t>
+  </si>
+  <si>
     <t>assuntos PRINCÍPIO DA INSIGNIFICÂNCIA</t>
   </si>
   <si>
-    <t>assuntos EXECUÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>origem_PB - PARAÍBA</t>
-  </si>
-  <si>
-    <t>origem_MG - MINAS GERAIS</t>
-  </si>
-  <si>
-    <t>origem_RO - RONDÔNIA</t>
-  </si>
-  <si>
-    <t>origem_RR - RORAIMA</t>
-  </si>
-  <si>
-    <t>origem_RS - RIO GRANDE DO SUL</t>
-  </si>
-  <si>
-    <t>origem_PI - PIAUÍ</t>
-  </si>
-  <si>
-    <t>origem_PE - PERNAMBUCO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>origem_RJ - RIO DE JANEIRO</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
-  </si>
-  <si>
-    <t>assuntos FIANÇA</t>
-  </si>
-  <si>
-    <t>origem_TO - TOCANTINS</t>
-  </si>
-  <si>
-    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
-  </si>
-  <si>
-    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
-  </si>
-  <si>
-    <t>assuntos REGRESSÃO DE REGIME</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
-  </si>
-  <si>
-    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES HEDIONDOS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
-  </si>
-  <si>
-    <t>assuntos EMPRESAS</t>
-  </si>
-  <si>
-    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos TRATAMENTO AMBULATORIAL</t>
-  </si>
-  <si>
-    <t>assuntos PRESCRIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos IMPEDIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos MANDATO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
-  </si>
-  <si>
-    <t>assuntos PROGRESSÃO DE REGIME</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A VIDA</t>
-  </si>
-  <si>
-    <t>assuntos REGIME INICIAL</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos QUADRILHA OU BANDO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos ABOLITIO CRIMINIS</t>
-  </si>
-  <si>
-    <t>Relator_CEZAR PELUSO</t>
-  </si>
-  <si>
-    <t>assuntos ESTRANGEIRO</t>
-  </si>
-  <si>
-    <t>origem_GO - GOIÁS</t>
-  </si>
-  <si>
-    <t>origem_AC - ACRE</t>
-  </si>
-  <si>
-    <t>origem_AM - AMAZONAS</t>
-  </si>
-  <si>
-    <t>origem_AP - AMAPÁ</t>
-  </si>
-  <si>
-    <t>origem_BA - BAHIA</t>
-  </si>
-  <si>
-    <t>origem_CE - CEARÁ</t>
-  </si>
-  <si>
-    <t>origem_DF - DISTRITO FEDERAL</t>
-  </si>
-  <si>
-    <t>origem_ES - ESPÍRITO SANTO</t>
-  </si>
-  <si>
-    <t>origem_MA - MARANHÃO</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>origem_MS - MATO GROSSO DO SUL</t>
-  </si>
-  <si>
-    <t>origem_MT - MATO GROSSO</t>
-  </si>
-  <si>
-    <t>origem_PA - PARÁ</t>
-  </si>
-  <si>
-    <t>origem_PR - PARANÁ</t>
-  </si>
-  <si>
-    <t>origem_RN - RIO GRANDE DO NORTE</t>
-  </si>
-  <si>
-    <t>origem_SC - SANTA CATARINA</t>
-  </si>
-  <si>
-    <t>origem_SE - SERGIPE</t>
-  </si>
-  <si>
-    <t>Relator_TEORI ZAVASCKI</t>
-  </si>
-  <si>
-    <t>Relator_OCTAVIO GALLOTTI</t>
-  </si>
-  <si>
-    <t>Relator_MOREIRA ALVES</t>
-  </si>
-  <si>
-    <t>Relator_JOAQUIM BARBOSA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
-  </si>
-  <si>
-    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
-  </si>
-  <si>
-    <t>Relator_ALEXANDRE DE MORAES</t>
-  </si>
-  <si>
-    <t>Relator_AYRES BRITTO</t>
-  </si>
-  <si>
-    <t>Relator_CARLOS VELLOSO</t>
-  </si>
-  <si>
-    <t>Relator_CELSO DE MELLO</t>
-  </si>
-  <si>
-    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>Relator_EDSON FACHIN</t>
-  </si>
-  <si>
-    <t>Relator_ELLEN GRACIE</t>
-  </si>
-  <si>
-    <t>Relator_EROS GRAU</t>
-  </si>
-  <si>
-    <t>Relator_FRANCISCO REZEK</t>
-  </si>
-  <si>
-    <t>Relator_GILMAR MENDES</t>
-  </si>
-  <si>
-    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
-  </si>
-  <si>
-    <t>Relator_ILMAR GALVÃO</t>
-  </si>
-  <si>
-    <t>assuntos PREFEITO</t>
-  </si>
-  <si>
-    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
-  </si>
-  <si>
-    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO EM FLAGRANTE</t>
-  </si>
-  <si>
-    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos NULIDADE OU ANULAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
-  </si>
-  <si>
-    <t>assuntos PROVAS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO CIVIL</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO (ART. 157)</t>
-  </si>
-  <si>
-    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
-  </si>
-  <si>
-    <t>assuntos RECEPTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
-  </si>
-  <si>
-    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos ELEIÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos JURISDIÇÃO E COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
-  </si>
-  <si>
-    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos FURTO</t>
-  </si>
-  <si>
-    <t>assuntos PARTE GERAL</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>DESCONHECIDO</t>
-  </si>
-  <si>
-    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>assuntos AFASTAMENTO DO CARGO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos CORRUPÇÃO PASSIVA</t>
-  </si>
-  <si>
-    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos EXTRADIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>assuntos RECURSO</t>
-  </si>
-  <si>
-    <t>assuntos INDULTO</t>
-  </si>
-  <si>
-    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO</t>
-  </si>
-  <si>
-    <t>assuntos HOMICÍDIO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DO MP</t>
-  </si>
-  <si>
-    <t>assuntos TRIBUNAL DE CONTAS</t>
-  </si>
-  <si>
-    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A PAZ PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES MILITARES</t>
-  </si>
-  <si>
-    <t>assuntos FATOS JURÍDICOS</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos ASSUNTOS DIVERSOS</t>
-  </si>
-  <si>
-    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos TIPICIDADE</t>
-  </si>
-  <si>
-    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos PROVA ILÍCITA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
+    <t>assuntos FURTO (ART. 155)</t>
   </si>
   <si>
     <t>assuntos SUSPEIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos FURTO (ART. 155)</t>
-  </si>
-  <si>
-    <t>assuntos Desconhecido</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ELEITORAL</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
-  </si>
-  <si>
-    <t>assuntos MEDIDAS DE SEGURANÇA</t>
-  </si>
-  <si>
-    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ELEITORAL E PROCESSO ELEITORAL</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS</t>
-  </si>
-  <si>
-    <t>assuntos DENEGAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO TEMPORÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
-  </si>
-  <si>
-    <t>assuntos SUSPENSÃO</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos INDEFERIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
-  </si>
-  <si>
-    <t>assuntos AGENTES POLÍTICOS</t>
-  </si>
-  <si>
-    <t>assuntos ESTELIONATO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos CERCEAMENTO DE DEFESA</t>
-  </si>
-  <si>
-    <t>assuntos APLICAÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos DENÚNCIA/QUEIXA</t>
-  </si>
-  <si>
-    <t>assuntos ATO INFRACIONAL</t>
-  </si>
-  <si>
-    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
-  </si>
-  <si>
-    <t>assuntos DESCLASSIFICAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A VIDA</t>
-  </si>
-  <si>
-    <t>assuntos LICITAÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos INSERÇÃO DE DADOS FALSOS EM SISTEMA DE INFORMAÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos ATOS PROCESSUAIS</t>
-  </si>
-  <si>
-    <t>assuntos RECEPTAÇÃO QUALIFICADA</t>
-  </si>
-  <si>
-    <t>assuntos RECUPERAÇÃO JUDICIAL E FALÊNCIA</t>
   </si>
   <si>
     <t>assuntos FURTO DE COISA COMUM</t>
@@ -1002,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.07000000000000001</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.07000000000000001</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1530,7 +1530,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1538,7 +1538,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1546,7 +1546,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1554,7 +1554,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="72" spans="1:2">

</xml_diff>

<commit_message>
Adj in model selection
</commit_message>
<xml_diff>
--- a/modeling/results/feature_imp_attr.xlsx
+++ b/modeling/results/feature_imp_attr.xlsx
@@ -25,429 +25,597 @@
     <t>diff_datas</t>
   </si>
   <si>
+    <t>CRIME DA LEI DE DROGAS</t>
+  </si>
+  <si>
+    <t>origem_SP - SÃO PAULO</t>
+  </si>
+  <si>
+    <t>Quant</t>
+  </si>
+  <si>
+    <t>assuntos JURISDIÇÃO E COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE</t>
+  </si>
+  <si>
+    <t>assuntos INVESTIGAÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>assuntos REVOGAÇÃO</t>
+  </si>
+  <si>
+    <t>Relator_CELSO DE MELLO</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>origem_AP - AMAPÁ</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO TEMPORÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos CERCEAMENTO DE DEFESA</t>
+  </si>
+  <si>
+    <t>assuntos LIBERDADE PROVISÓRIA</t>
+  </si>
+  <si>
+    <t>Relator_JOAQUIM BARBOSA</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>Relator_LUIZ FUX</t>
+  </si>
+  <si>
+    <t>Relator_MARCO AURÉLIO</t>
+  </si>
+  <si>
+    <t>Relator_CEZAR PELUSO</t>
+  </si>
+  <si>
+    <t>Relator_AYRES BRITTO</t>
+  </si>
+  <si>
+    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
+  </si>
+  <si>
+    <t>Relator_CARLOS VELLOSO</t>
+  </si>
+  <si>
+    <t>assuntos ATOS PROCESSUAIS</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A PESSOA</t>
+  </si>
+  <si>
+    <t>assuntos LICITAÇÕES</t>
+  </si>
+  <si>
+    <t>Relator_CÁRMEN LÚCIA</t>
+  </si>
+  <si>
+    <t>Relator_DIAS TOFFOLI</t>
+  </si>
+  <si>
+    <t>Relator_ALEXANDRE DE MORAES</t>
+  </si>
+  <si>
+    <t>Relator_EDSON FACHIN</t>
+  </si>
+  <si>
+    <t>assuntos DENÚNCIA/QUEIXA</t>
+  </si>
+  <si>
+    <t>Relator_GILMAR MENDES</t>
+  </si>
+  <si>
+    <t>Relator_ILMAR GALVÃO</t>
+  </si>
+  <si>
+    <t>assuntos DESCLASSIFICAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
+  </si>
+  <si>
+    <t>Relator_MOREIRA ALVES</t>
+  </si>
+  <si>
+    <t>assuntos QUADRILHA OU BANDO</t>
+  </si>
+  <si>
+    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos LIVRAMENTO CONDICIONAL</t>
+  </si>
+  <si>
+    <t>assuntos PROGRESSÃO DE REGIME</t>
+  </si>
+  <si>
+    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A VIDA</t>
+  </si>
+  <si>
+    <t>assuntos REGRESSÃO DE REGIME</t>
+  </si>
+  <si>
+    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos PRESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
+  </si>
+  <si>
+    <t>assuntos MEDIDAS DE SEGURANÇA</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
+  </si>
+  <si>
+    <t>CRIME DA LEI DE ARMAS</t>
+  </si>
+  <si>
+    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
+  </si>
+  <si>
+    <t>assuntos PRINCÍPIO DA INSIGNIFICÂNCIA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
+  </si>
+  <si>
+    <t>assuntos PROVA ILÍCITA</t>
+  </si>
+  <si>
+    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos ESTRANGEIRO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
+  </si>
+  <si>
+    <t>assuntos SUSPENSÃO</t>
+  </si>
+  <si>
+    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
+  </si>
+  <si>
+    <t>Relator_OCTAVIO GALLOTTI</t>
+  </si>
+  <si>
+    <t>origem_RR - RORAIMA</t>
+  </si>
+  <si>
+    <t>origem_PE - PERNAMBUCO</t>
+  </si>
+  <si>
+    <t>origem_PI - PIAUÍ</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO</t>
+  </si>
+  <si>
+    <t>assuntos DENEGAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos FIANÇA</t>
+  </si>
+  <si>
+    <t>assuntos INDULTO</t>
+  </si>
+  <si>
+    <t>assuntos RECURSO</t>
+  </si>
+  <si>
+    <t>origem_RN - RIO GRANDE DO NORTE</t>
+  </si>
+  <si>
+    <t>origem_RO - RONDÔNIA</t>
+  </si>
+  <si>
+    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
+  </si>
+  <si>
+    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
+  </si>
+  <si>
+    <t>origem_PB - PARAÍBA</t>
+  </si>
+  <si>
+    <t>origem_SC - SANTA CATARINA</t>
+  </si>
+  <si>
+    <t>origem_SE - SERGIPE</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
+  </si>
+  <si>
+    <t>DESCONHECIDO</t>
+  </si>
+  <si>
+    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO EM FLAGRANTE</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
+  </si>
+  <si>
+    <t>origem_PA - PARÁ</t>
+  </si>
+  <si>
+    <t>origem_MA - MARANHÃO</t>
+  </si>
+  <si>
+    <t>origem_AC - ACRE</t>
+  </si>
+  <si>
+    <t>Relator_TEORI ZAVASCKI</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO CIVIL</t>
+  </si>
+  <si>
+    <t>Relator_ROBERTO BARROSO</t>
+  </si>
+  <si>
+    <t>origem_CE - CEARÁ</t>
+  </si>
+  <si>
+    <t>assuntos PROVAS</t>
+  </si>
+  <si>
+    <t>origem_MG - MINAS GERAIS</t>
+  </si>
+  <si>
+    <t>origem_MS - MATO GROSSO DO SUL</t>
+  </si>
+  <si>
+    <t>Relator_RICARDO LEWANDOWSKI</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
+  </si>
+  <si>
+    <t>origem_DF - DISTRITO FEDERAL</t>
+  </si>
+  <si>
+    <t>Relator_EROS GRAU</t>
+  </si>
+  <si>
+    <t>Relator_FRANCISCO REZEK</t>
+  </si>
+  <si>
+    <t>origem_AL - ALAGOAS</t>
+  </si>
+  <si>
+    <t>origem_TO - TOCANTINS</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>assuntos MANDATO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
+  </si>
+  <si>
+    <t>assuntos TRATAMENTO AMBULATORIAL</t>
+  </si>
+  <si>
+    <t>Relator_ROSA WEBER</t>
+  </si>
+  <si>
+    <t>assuntos REGIME INICIAL</t>
+  </si>
+  <si>
+    <t>origem_AM - AMAZONAS</t>
+  </si>
+  <si>
+    <t>origem_RS - RIO GRANDE DO SUL</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
+  </si>
+  <si>
     <t>assuntos PRISÃO PREVENTIVA</t>
   </si>
   <si>
-    <t>Relator_MARCO AURÉLIO</t>
-  </si>
-  <si>
-    <t>origem_SP - SÃO PAULO</t>
-  </si>
-  <si>
-    <t>assuntos REVOGAÇÃO</t>
-  </si>
-  <si>
-    <t>Relator_JOAQUIM BARBOSA</t>
-  </si>
-  <si>
-    <t>assuntos LIBERDADE PROVISÓRIA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A VIDA</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
-  </si>
-  <si>
-    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos PROGRESSÃO DE REGIME</t>
-  </si>
-  <si>
-    <t>assuntos LIVRAMENTO CONDICIONAL</t>
-  </si>
-  <si>
-    <t>assuntos REGIME INICIAL</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
+    <t>assuntos CRIMES HEDIONDOS</t>
+  </si>
+  <si>
+    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
+  </si>
+  <si>
+    <t>Relator_ELLEN GRACIE</t>
+  </si>
+  <si>
+    <t>origem_BA - BAHIA</t>
+  </si>
+  <si>
+    <t>origem_ES - ESPÍRITO SANTO</t>
+  </si>
+  <si>
+    <t>origem_RJ - RIO DE JANEIRO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>origem_GO - GOIÁS</t>
+  </si>
+  <si>
+    <t>assuntos ABOLITIO CRIMINIS</t>
+  </si>
+  <si>
+    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>origem_MT - MATO GROSSO</t>
+  </si>
+  <si>
+    <t>origem_PR - PARANÁ</t>
+  </si>
+  <si>
+    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO (ART. 157)</t>
+  </si>
+  <si>
+    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
+  </si>
+  <si>
+    <t>assuntos RECEPTAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
+  </si>
+  <si>
+    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos ELEIÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos HOMICÍDIO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos FURTO</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DO MP</t>
+  </si>
+  <si>
+    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
+  </si>
+  <si>
+    <t>assuntos FURTO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos AFASTAMENTO DO CARGO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos CORRUPÇÃO PASSIVA</t>
+  </si>
+  <si>
+    <t>assuntos EXTRADIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
+  </si>
+  <si>
+    <t>assuntos PARTE GERAL</t>
+  </si>
+  <si>
+    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
+  </si>
+  <si>
+    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE OU ANULAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos INDEFERIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos AGENTES POLÍTICOS</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL</t>
+  </si>
+  <si>
+    <t>assuntos TIPICIDADE</t>
+  </si>
+  <si>
+    <t>assuntos SUSPEIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos FURTO (ART. 155)</t>
+  </si>
+  <si>
+    <t>assuntos Desconhecido</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO MAJORADO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ELEITORAL</t>
+  </si>
+  <si>
+    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
+  </si>
+  <si>
+    <t>assuntos TRIBUNAL DE CONTAS</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
   </si>
   <si>
     <t>assuntos PREFEITO</t>
   </si>
   <si>
-    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ELEITORAL</t>
-  </si>
-  <si>
-    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
-  </si>
-  <si>
-    <t>assuntos PROVA ILÍCITA</t>
-  </si>
-  <si>
-    <t>assuntos TIPICIDADE</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO TEMPORÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos ATOS PROCESSUAIS</t>
-  </si>
-  <si>
-    <t>assuntos LICITAÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos DESCLASSIFICAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
-  </si>
-  <si>
-    <t>Relator_AYRES BRITTO</t>
-  </si>
-  <si>
-    <t>assuntos NULIDADE</t>
-  </si>
-  <si>
-    <t>assuntos CERCEAMENTO DE DEFESA</t>
-  </si>
-  <si>
-    <t>origem_SC - SANTA CATARINA</t>
-  </si>
-  <si>
-    <t>origem_RR - RORAIMA</t>
-  </si>
-  <si>
-    <t>origem_RO - RONDÔNIA</t>
-  </si>
-  <si>
-    <t>origem_RN - RIO GRANDE DO NORTE</t>
-  </si>
-  <si>
-    <t>origem_PE - PERNAMBUCO</t>
-  </si>
-  <si>
-    <t>origem_PB - PARAÍBA</t>
-  </si>
-  <si>
-    <t>origem_MS - MATO GROSSO DO SUL</t>
-  </si>
-  <si>
-    <t>origem_ES - ESPÍRITO SANTO</t>
-  </si>
-  <si>
-    <t>origem_CE - CEARÁ</t>
-  </si>
-  <si>
-    <t>origem_AP - AMAPÁ</t>
-  </si>
-  <si>
-    <t>origem_AC - ACRE</t>
-  </si>
-  <si>
-    <t>Relator_TEORI ZAVASCKI</t>
-  </si>
-  <si>
-    <t>Relator_ROBERTO BARROSO</t>
-  </si>
-  <si>
-    <t>Relator_RICARDO LEWANDOWSKI</t>
-  </si>
-  <si>
-    <t>Relator_OCTAVIO GALLOTTI</t>
-  </si>
-  <si>
-    <t>Relator_MOREIRA ALVES</t>
-  </si>
-  <si>
-    <t>Relator_LUIZ FUX</t>
-  </si>
-  <si>
-    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
-  </si>
-  <si>
-    <t>Relator_DIAS TOFFOLI</t>
-  </si>
-  <si>
-    <t>Relator_CÁRMEN LÚCIA</t>
-  </si>
-  <si>
-    <t>Relator_CEZAR PELUSO</t>
-  </si>
-  <si>
-    <t>Relator_CELSO DE MELLO</t>
-  </si>
-  <si>
-    <t>Relator_CARLOS VELLOSO</t>
-  </si>
-  <si>
-    <t>assuntos INVESTIGAÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>Quant</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
-  </si>
-  <si>
-    <t>assuntos EXECUÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>CRIME DA LEI DE ARMAS</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A PESSOA</t>
-  </si>
-  <si>
-    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
-  </si>
-  <si>
-    <t>assuntos INDULTO</t>
-  </si>
-  <si>
-    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos FIANÇA</t>
-  </si>
-  <si>
-    <t>Relator_ALEXANDRE DE MORAES</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
-  </si>
-  <si>
-    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO</t>
-  </si>
-  <si>
-    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
-  </si>
-  <si>
-    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>Relator_EDSON FACHIN</t>
-  </si>
-  <si>
-    <t>Relator_ELLEN GRACIE</t>
-  </si>
-  <si>
-    <t>Relator_EROS GRAU</t>
-  </si>
-  <si>
-    <t>assuntos RECURSO</t>
-  </si>
-  <si>
-    <t>assuntos ESTRANGEIRO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>Relator_GILMAR MENDES</t>
-  </si>
-  <si>
-    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos ABOLITIO CRIMINIS</t>
-  </si>
-  <si>
-    <t>assuntos PARTE GERAL</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO EM FLAGRANTE</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES HEDIONDOS</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
-  </si>
-  <si>
-    <t>assuntos TRATAMENTO AMBULATORIAL</t>
-  </si>
-  <si>
-    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos PRESCRIÇÃO</t>
-  </si>
-  <si>
-    <t>Relator_FRANCISCO REZEK</t>
-  </si>
-  <si>
-    <t>assuntos EXTRADIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>Relator_ILMAR GALVÃO</t>
-  </si>
-  <si>
-    <t>origem_TO - TOCANTINS</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>origem_SE - SERGIPE</t>
-  </si>
-  <si>
-    <t>origem_RS - RIO GRANDE DO SUL</t>
-  </si>
-  <si>
-    <t>CRIME DA LEI DE DROGAS</t>
-  </si>
-  <si>
-    <t>origem_RJ - RIO DE JANEIRO</t>
-  </si>
-  <si>
-    <t>origem_PR - PARANÁ</t>
-  </si>
-  <si>
-    <t>origem_PI - PIAUÍ</t>
-  </si>
-  <si>
-    <t>origem_PA - PARÁ</t>
-  </si>
-  <si>
-    <t>origem_MT - MATO GROSSO</t>
-  </si>
-  <si>
-    <t>DESCONHECIDO</t>
-  </si>
-  <si>
-    <t>origem_MG - MINAS GERAIS</t>
-  </si>
-  <si>
-    <t>origem_MA - MARANHÃO</t>
-  </si>
-  <si>
-    <t>origem_GO - GOIÁS</t>
-  </si>
-  <si>
-    <t>origem_DF - DISTRITO FEDERAL</t>
-  </si>
-  <si>
-    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>origem_BA - BAHIA</t>
-  </si>
-  <si>
-    <t>origem_AM - AMAZONAS</t>
-  </si>
-  <si>
-    <t>origem_AL - ALAGOAS</t>
-  </si>
-  <si>
-    <t>assuntos AFASTAMENTO DO CARGO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>Relator_ROSA WEBER</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos CORRUPÇÃO PASSIVA</t>
-  </si>
-  <si>
-    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos MANDATO</t>
-  </si>
-  <si>
-    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
-  </si>
-  <si>
-    <t>assuntos FURTO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
+    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
+  </si>
+  <si>
+    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
+  </si>
+  <si>
+    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos EMPRESAS</t>
+  </si>
+  <si>
+    <t>assuntos IMPEDIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
+  </si>
+  <si>
+    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos ESTELIONATO MAJORADO</t>
+  </si>
+  <si>
+    <t>assuntos ASSUNTOS DIVERSOS</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL PENAL</t>
+  </si>
+  <si>
+    <t>assuntos TRANCAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos APLICAÇÃO DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos ATO INFRACIONAL</t>
+  </si>
+  <si>
+    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA A VIDA</t>
+  </si>
+  <si>
+    <t>assuntos PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
   </si>
   <si>
     <t>assuntos INSERÇÃO DE DADOS FALSOS EM SISTEMA DE INFORMAÇÕES</t>
   </si>
   <si>
-    <t>assuntos JURISDIÇÃO E COMPETÊNCIA</t>
-  </si>
-  <si>
     <t>assuntos RECEPTAÇÃO QUALIFICADA</t>
   </si>
   <si>
     <t>assuntos RECUPERAÇÃO JUDICIAL E FALÊNCIA</t>
   </si>
   <si>
-    <t>assuntos ELEIÇÕES</t>
-  </si>
-  <si>
     <t>assuntos HABEAS CORPUS</t>
   </si>
   <si>
     <t>assuntos DIREITO ELEITORAL E PROCESSO ELEITORAL</t>
   </si>
   <si>
-    <t>assuntos PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
-  </si>
-  <si>
     <t>assuntos CRIMES CONTRA A PAZ PÚBLICA</t>
   </si>
   <si>
@@ -455,174 +623,6 @@
   </si>
   <si>
     <t>assuntos FATOS JURÍDICOS</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos ASSUNTOS DIVERSOS</t>
-  </si>
-  <si>
-    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos HOMICÍDIO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A VIDA</t>
-  </si>
-  <si>
-    <t>assuntos NULIDADE OU ANULAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL PENAL</t>
-  </si>
-  <si>
-    <t>assuntos SUSPENSÃO</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos INDEFERIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
-  </si>
-  <si>
-    <t>assuntos AGENTES POLÍTICOS</t>
-  </si>
-  <si>
-    <t>assuntos ESTELIONATO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos DENEGAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos FURTO</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DO MP</t>
-  </si>
-  <si>
-    <t>assuntos TRANCAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos APLICAÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos DENÚNCIA/QUEIXA</t>
-  </si>
-  <si>
-    <t>assuntos ATO INFRACIONAL</t>
-  </si>
-  <si>
-    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos IMPEDIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos REGRESSÃO DE REGIME</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO CIVIL</t>
-  </si>
-  <si>
-    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos EMPRESAS</t>
-  </si>
-  <si>
-    <t>assuntos PROVAS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
-  </si>
-  <si>
-    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos QUADRILHA OU BANDO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO (ART. 157)</t>
-  </si>
-  <si>
-    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos TRIBUNAL DE CONTAS</t>
-  </si>
-  <si>
-    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
-  </si>
-  <si>
-    <t>assuntos MEDIDAS DE SEGURANÇA</t>
-  </si>
-  <si>
-    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
-  </si>
-  <si>
-    <t>assuntos RECEPTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
-  </si>
-  <si>
-    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos Desconhecido</t>
-  </si>
-  <si>
-    <t>assuntos PRINCÍPIO DA INSIGNIFICÂNCIA</t>
-  </si>
-  <si>
-    <t>assuntos FURTO (ART. 155)</t>
-  </si>
-  <si>
-    <t>assuntos SUSPEIÇÃO</t>
   </si>
   <si>
     <t>assuntos FURTO DE COISA COMUM</t>
@@ -1002,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.23</v>
+        <v>0.45703125</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
+        <v>0.05859375</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.02</v>
+        <v>0.01953125</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.02</v>
+        <v>0.01171875</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.02</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.02</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.01</v>
+        <v>0.0078125</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1170,7 +1170,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1210,7 +1210,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1218,7 +1218,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1266,7 +1266,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1298,7 +1298,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1530,7 +1530,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1538,7 +1538,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1546,7 +1546,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1554,7 +1554,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>0.01</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1562,7 +1562,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1570,7 +1570,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1578,7 +1578,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1586,7 +1586,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1594,7 +1594,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1602,7 +1602,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1610,7 +1610,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1618,7 +1618,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1626,7 +1626,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1634,7 +1634,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1642,7 +1642,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1650,7 +1650,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1658,7 +1658,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1666,7 +1666,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1674,7 +1674,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1698,7 +1698,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1706,7 +1706,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1714,7 +1714,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1730,7 +1730,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1738,7 +1738,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1746,7 +1746,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1754,7 +1754,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1762,7 +1762,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1770,7 +1770,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1778,7 +1778,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1786,7 +1786,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>0.00390625</v>
       </c>
     </row>
     <row r="101" spans="1:2">

</xml_diff>

<commit_message>
Adjustments in final results and modelling
</commit_message>
<xml_diff>
--- a/modeling/results/feature_imp_attr.xlsx
+++ b/modeling/results/feature_imp_attr.xlsx
@@ -25,604 +25,604 @@
     <t>diff_datas</t>
   </si>
   <si>
+    <t>Quant</t>
+  </si>
+  <si>
+    <t>Relator_MARCO AURÉLIO</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A PESSOA</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO PREVENTIVA</t>
+  </si>
+  <si>
     <t>CRIME DA LEI DE DROGAS</t>
   </si>
   <si>
+    <t>origem_PE - PERNAMBUCO</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>origem_PR - PARANÁ</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
+  </si>
+  <si>
     <t>origem_SP - SÃO PAULO</t>
   </si>
   <si>
-    <t>Quant</t>
+    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
+  </si>
+  <si>
+    <t>origem_MS - MATO GROSSO DO SUL</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
+  </si>
+  <si>
+    <t>assuntos LIBERDADE PROVISÓRIA</t>
+  </si>
+  <si>
+    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>Relator_RICARDO LEWANDOWSKI</t>
+  </si>
+  <si>
+    <t>origem_MG - MINAS GERAIS</t>
+  </si>
+  <si>
+    <t>Relator_CELSO DE MELLO</t>
+  </si>
+  <si>
+    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>Relator_EDSON FACHIN</t>
+  </si>
+  <si>
+    <t>Relator_CÁRMEN LÚCIA</t>
+  </si>
+  <si>
+    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>origem_PI - PIAUÍ</t>
+  </si>
+  <si>
+    <t>origem_RN - RIO GRANDE DO NORTE</t>
+  </si>
+  <si>
+    <t>origem_CE - CEARÁ</t>
+  </si>
+  <si>
+    <t>assuntos REVOGAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
+  </si>
+  <si>
+    <t>origem_MA - MARANHÃO</t>
+  </si>
+  <si>
+    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
+  </si>
+  <si>
+    <t>assuntos TIPICIDADE</t>
+  </si>
+  <si>
+    <t>origem_RS - RIO GRANDE DO SUL</t>
+  </si>
+  <si>
+    <t>origem_RJ - RIO DE JANEIRO</t>
+  </si>
+  <si>
+    <t>Relator_ROSA WEBER</t>
+  </si>
+  <si>
+    <t>origem_SE - SERGIPE</t>
+  </si>
+  <si>
+    <t>Relator_ROBERTO BARROSO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
+  </si>
+  <si>
+    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
   </si>
   <si>
     <t>assuntos JURISDIÇÃO E COMPETÊNCIA</t>
   </si>
   <si>
-    <t>assuntos NULIDADE</t>
+    <t>Relator_AYRES BRITTO</t>
+  </si>
+  <si>
+    <t>assuntos PRINCÍPIO DA INSIGNIFICÂNCIA</t>
+  </si>
+  <si>
+    <t>Relator_TEORI ZAVASCKI</t>
+  </si>
+  <si>
+    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
+  </si>
+  <si>
+    <t>origem_DF - DISTRITO FEDERAL</t>
+  </si>
+  <si>
+    <t>CRIME DA LEI DE ARMAS</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL</t>
+  </si>
+  <si>
+    <t>Relator_DIAS TOFFOLI</t>
+  </si>
+  <si>
+    <t>origem_AL - ALAGOAS</t>
+  </si>
+  <si>
+    <t>Relator_GILMAR MENDES</t>
+  </si>
+  <si>
+    <t>DESCONHECIDO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL</t>
+  </si>
+  <si>
+    <t>origem_SC - SANTA CATARINA</t>
+  </si>
+  <si>
+    <t>Relator_LUIZ FUX</t>
+  </si>
+  <si>
+    <t>assuntos REGIME INICIAL</t>
+  </si>
+  <si>
+    <t>origem_AP - AMAPÁ</t>
+  </si>
+  <si>
+    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
+  </si>
+  <si>
+    <t>origem_MT - MATO GROSSO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos SUSPENSÃO</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL PENAL</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO EM FLAGRANTE</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ELEITORAL</t>
+  </si>
+  <si>
+    <t>origem_PA - PARÁ</t>
+  </si>
+  <si>
+    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos RECURSO</t>
+  </si>
+  <si>
+    <t>assuntos PRISÃO TEMPORÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>Relator_ILMAR GALVÃO</t>
+  </si>
+  <si>
+    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos DESCLASSIFICAÇÃO</t>
+  </si>
+  <si>
+    <t>Relator_ALEXANDRE DE MORAES</t>
+  </si>
+  <si>
+    <t>Relator_JOAQUIM BARBOSA</t>
+  </si>
+  <si>
+    <t>Relator_OCTAVIO GALLOTTI</t>
+  </si>
+  <si>
+    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
+  </si>
+  <si>
+    <t>origem_RO - RONDÔNIA</t>
+  </si>
+  <si>
+    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
+  </si>
+  <si>
+    <t>assuntos TRATAMENTO AMBULATORIAL</t>
+  </si>
+  <si>
+    <t>origem_PB - PARAÍBA</t>
+  </si>
+  <si>
+    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
+  </si>
+  <si>
+    <t>origem_RR - RORAIMA</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO</t>
+  </si>
+  <si>
+    <t>assuntos CERCEAMENTO DE DEFESA</t>
+  </si>
+  <si>
+    <t>Relator_CEZAR PELUSO</t>
+  </si>
+  <si>
+    <t>Relator_MOREIRA ALVES</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
+  </si>
+  <si>
+    <t>assuntos DENEGAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos APLICAÇÃO DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>Relator_ELLEN GRACIE</t>
+  </si>
+  <si>
+    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
+  </si>
+  <si>
+    <t>assuntos INDULTO</t>
+  </si>
+  <si>
+    <t>origem_AC - ACRE</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
+  </si>
+  <si>
+    <t>assuntos FIANÇA</t>
+  </si>
+  <si>
+    <t>assuntos EMPRESAS</t>
   </si>
   <si>
     <t>assuntos INVESTIGAÇÃO PENAL</t>
   </si>
   <si>
-    <t>assuntos REVOGAÇÃO</t>
-  </si>
-  <si>
-    <t>Relator_CELSO DE MELLO</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos EXECUÇÃO PENAL</t>
-  </si>
-  <si>
-    <t>origem_AP - AMAPÁ</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO TEMPORÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos CERCEAMENTO DE DEFESA</t>
-  </si>
-  <si>
-    <t>assuntos LIBERDADE PROVISÓRIA</t>
-  </si>
-  <si>
-    <t>Relator_JOAQUIM BARBOSA</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A INCOLUMIDADE PAZ E FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>Relator_LUIZ FUX</t>
-  </si>
-  <si>
-    <t>Relator_MARCO AURÉLIO</t>
-  </si>
-  <si>
-    <t>Relator_CEZAR PELUSO</t>
-  </si>
-  <si>
-    <t>Relator_AYRES BRITTO</t>
-  </si>
-  <si>
-    <t>assuntos CONSTRANGIMENTO ILEGAL</t>
+    <t>assuntos EXTRADIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A VIDA</t>
   </si>
   <si>
     <t>Relator_CARLOS VELLOSO</t>
   </si>
   <si>
+    <t>assuntos PROVA ILÍCITA</t>
+  </si>
+  <si>
+    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
+  </si>
+  <si>
+    <t>assuntos LIVRAMENTO CONDICIONAL</t>
+  </si>
+  <si>
+    <t>assuntos PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
+  </si>
+  <si>
+    <t>assuntos TRANCAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos ABOLITIO CRIMINIS</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DO MP</t>
+  </si>
+  <si>
+    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO (ART. 157)</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO CIVIL</t>
+  </si>
+  <si>
+    <t>origem_TO - TOCANTINS</t>
+  </si>
+  <si>
+    <t>assuntos AFASTAMENTO DO CARGO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos CORRUPÇÃO PASSIVA</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>origem_AM - AMAZONAS</t>
+  </si>
+  <si>
+    <t>assuntos PROVAS</t>
+  </si>
+  <si>
+    <t>assuntos NULIDADE OU ANULAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
+  </si>
+  <si>
+    <t>origem_BA - BAHIA</t>
+  </si>
+  <si>
+    <t>origem_ES - ESPÍRITO SANTO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
+  </si>
+  <si>
+    <t>origem_GO - GOIÁS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
+  </si>
+  <si>
+    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
+  </si>
+  <si>
+    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
+  </si>
+  <si>
+    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
+  </si>
+  <si>
+    <t>Relator_FRANCISCO REZEK</t>
+  </si>
+  <si>
+    <t>Relator_EROS GRAU</t>
+  </si>
+  <si>
+    <t>assuntos PARTE GERAL</t>
+  </si>
+  <si>
+    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos ESTELIONATO MAJORADO</t>
+  </si>
+  <si>
+    <t>assuntos ESTRANGEIRO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES MILITARES</t>
+  </si>
+  <si>
+    <t>assuntos Desconhecido</t>
+  </si>
+  <si>
+    <t>assuntos INDEFERIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos FURTO (ART. 155)</t>
+  </si>
+  <si>
+    <t>assuntos SUSPEIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
+  </si>
+  <si>
+    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
+  </si>
+  <si>
+    <t>assuntos AGENTES POLÍTICOS</t>
+  </si>
+  <si>
+    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos ASSUNTOS DIVERSOS</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS ELEITORAIS</t>
+  </si>
+  <si>
+    <t>assuntos FATOS JURÍDICOS</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A PAZ PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos AÇÃO PENAL MILITAR</t>
+  </si>
+  <si>
+    <t>assuntos DIREITO ELEITORAL E PROCESSO ELEITORAL</t>
+  </si>
+  <si>
+    <t>assuntos HABEAS CORPUS</t>
+  </si>
+  <si>
+    <t>assuntos RECUPERAÇÃO JUDICIAL E FALÊNCIA</t>
+  </si>
+  <si>
+    <t>assuntos RECEPTAÇÃO QUALIFICADA</t>
+  </si>
+  <si>
     <t>assuntos ATOS PROCESSUAIS</t>
   </si>
   <si>
-    <t>CRIME CONTRA A PESSOA</t>
+    <t>assuntos INSERÇÃO DE DADOS FALSOS EM SISTEMA DE INFORMAÇÕES</t>
   </si>
   <si>
     <t>assuntos LICITAÇÕES</t>
   </si>
   <si>
-    <t>Relator_CÁRMEN LÚCIA</t>
-  </si>
-  <si>
-    <t>Relator_DIAS TOFFOLI</t>
-  </si>
-  <si>
-    <t>Relator_ALEXANDRE DE MORAES</t>
-  </si>
-  <si>
-    <t>Relator_EDSON FACHIN</t>
+    <t>assuntos CONTRA A VIDA</t>
+  </si>
+  <si>
+    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
+  </si>
+  <si>
+    <t>assuntos ATO INFRACIONAL</t>
   </si>
   <si>
     <t>assuntos DENÚNCIA/QUEIXA</t>
   </si>
   <si>
-    <t>Relator_GILMAR MENDES</t>
-  </si>
-  <si>
-    <t>Relator_ILMAR GALVÃO</t>
-  </si>
-  <si>
-    <t>assuntos DESCLASSIFICAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE "LAVAGEM" OU OCULTAÇÃO DE BENS, DIREITOS OU VALORES</t>
-  </si>
-  <si>
-    <t>Relator_MOREIRA ALVES</t>
+    <t>assuntos ROUBO MAJORADO</t>
+  </si>
+  <si>
+    <t>assuntos FURTO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
+  </si>
+  <si>
+    <t>assuntos RECEPTAÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES HEDIONDOS</t>
+  </si>
+  <si>
+    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
+  </si>
+  <si>
+    <t>assuntos PRESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>assuntos MANDATO</t>
+  </si>
+  <si>
+    <t>assuntos PROGRESSÃO DE REGIME</t>
+  </si>
+  <si>
+    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
+  </si>
+  <si>
+    <t>assuntos CONTRA O PATRIMÔNIO</t>
+  </si>
+  <si>
+    <t>assuntos ROUBO QUALIFICADO</t>
   </si>
   <si>
     <t>assuntos QUADRILHA OU BANDO</t>
   </si>
   <si>
-    <t>assuntos EXCESSO DE PRAZO PARA INSTRUÇÃO / JULGAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos LIVRAMENTO CONDICIONAL</t>
-  </si>
-  <si>
-    <t>assuntos PROGRESSÃO DE REGIME</t>
-  </si>
-  <si>
-    <t>assuntos SUBSTITUIÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A VIDA</t>
+    <t>assuntos ELEIÇÕES</t>
+  </si>
+  <si>
+    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
+  </si>
+  <si>
+    <t>assuntos HOMICÍDIO QUALIFICADO</t>
+  </si>
+  <si>
+    <t>assuntos IMPEDIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos FURTO</t>
+  </si>
+  <si>
+    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
   </si>
   <si>
     <t>assuntos REGRESSÃO DE REGIME</t>
   </si>
   <si>
-    <t>assuntos COLABORAÇÃO COM GRUPO, ORGANIZAÇÃO OU ASSOCIAÇÃO DESTINADOS À PRODUÇÃO OU TRÁFICO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos PRESCRIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ADMINISTRATIVO E OUTRAS MATÉRIAS DE DIREITO PÚBLICO</t>
+    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
+  </si>
+  <si>
+    <t>assuntos PREFEITO</t>
+  </si>
+  <si>
+    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
+  </si>
+  <si>
+    <t>assuntos TRIBUNAL DE CONTAS</t>
+  </si>
+  <si>
+    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
   </si>
   <si>
     <t>assuntos MEDIDAS DE SEGURANÇA</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DOMICILIAR / ESPECIAL</t>
-  </si>
-  <si>
-    <t>CRIME DA LEI DE ARMAS</t>
-  </si>
-  <si>
-    <t>CRIME DE LAVAGEM OU OCULTAÇÃO DE BENS</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO DECORRENTE DE SENTENÇA CONDENATÓRIA</t>
-  </si>
-  <si>
-    <t>assuntos PRINCÍPIO DA INSIGNIFICÂNCIA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
-  </si>
-  <si>
-    <t>assuntos PROVA ILÍCITA</t>
-  </si>
-  <si>
-    <t>assuntos AUSÊNCIA DE FUNDAMENTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos ESTRANGEIRO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DO SISTEMA NACIONAL DE ARMAS</t>
-  </si>
-  <si>
-    <t>assuntos SUSPENSÃO</t>
-  </si>
-  <si>
-    <t>Relator_HERMINIO DO ESPIRITO SANTO</t>
-  </si>
-  <si>
-    <t>Relator_OCTAVIO GALLOTTI</t>
-  </si>
-  <si>
-    <t>origem_RR - RORAIMA</t>
-  </si>
-  <si>
-    <t>origem_PE - PERNAMBUCO</t>
-  </si>
-  <si>
-    <t>origem_PI - PIAUÍ</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO</t>
-  </si>
-  <si>
-    <t>assuntos DENEGAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos FIANÇA</t>
-  </si>
-  <si>
-    <t>assuntos INDULTO</t>
-  </si>
-  <si>
-    <t>assuntos RECURSO</t>
-  </si>
-  <si>
-    <t>origem_RN - RIO GRANDE DO NORTE</t>
-  </si>
-  <si>
-    <t>origem_RO - RONDÔNIA</t>
-  </si>
-  <si>
-    <t>assuntos PENA PRIVATIVA DE LIBERDADE</t>
-  </si>
-  <si>
-    <t>assuntos VÍCIO FORMAL DO JULGAMENTO</t>
-  </si>
-  <si>
-    <t>origem_PB - PARAÍBA</t>
-  </si>
-  <si>
-    <t>origem_SC - SANTA CATARINA</t>
-  </si>
-  <si>
-    <t>origem_SE - SERGIPE</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>CRIME DE ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA A DIGNIDADE SEXUAL</t>
-  </si>
-  <si>
-    <t>DESCONHECIDO</t>
-  </si>
-  <si>
-    <t>CRIME OUTROS DAS LEIS ESPECIAIS</t>
-  </si>
-  <si>
-    <t>CRIME CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO EM FLAGRANTE</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS - CABIMENTO</t>
-  </si>
-  <si>
-    <t>origem_PA - PARÁ</t>
-  </si>
-  <si>
-    <t>origem_MA - MARANHÃO</t>
-  </si>
-  <si>
-    <t>origem_AC - ACRE</t>
-  </si>
-  <si>
-    <t>Relator_TEORI ZAVASCKI</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO CIVIL</t>
-  </si>
-  <si>
-    <t>Relator_ROBERTO BARROSO</t>
-  </si>
-  <si>
-    <t>origem_CE - CEARÁ</t>
-  </si>
-  <si>
-    <t>assuntos PROVAS</t>
-  </si>
-  <si>
-    <t>origem_MG - MINAS GERAIS</t>
-  </si>
-  <si>
-    <t>origem_MS - MATO GROSSO DO SUL</t>
-  </si>
-  <si>
-    <t>Relator_RICARDO LEWANDOWSKI</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DA LEI DE LICITAÇÕES</t>
-  </si>
-  <si>
-    <t>origem_DF - DISTRITO FEDERAL</t>
-  </si>
-  <si>
-    <t>Relator_EROS GRAU</t>
-  </si>
-  <si>
-    <t>Relator_FRANCISCO REZEK</t>
-  </si>
-  <si>
-    <t>origem_AL - ALAGOAS</t>
-  </si>
-  <si>
-    <t>origem_TO - TOCANTINS</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA O PATRIMÔNIO</t>
-  </si>
-  <si>
-    <t>assuntos MANDATO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL CIVIL E DO TRABALHO</t>
-  </si>
-  <si>
-    <t>assuntos TRATAMENTO AMBULATORIAL</t>
-  </si>
-  <si>
-    <t>Relator_ROSA WEBER</t>
-  </si>
-  <si>
-    <t>assuntos REGIME INICIAL</t>
-  </si>
-  <si>
-    <t>origem_AM - AMAZONAS</t>
-  </si>
-  <si>
-    <t>origem_RS - RIO GRANDE DO SUL</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO DA CRIANÇA E DO ADOLESCENTE</t>
-  </si>
-  <si>
-    <t>assuntos PRISÃO PREVENTIVA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES HEDIONDOS</t>
-  </si>
-  <si>
-    <t>assuntos TRANSFERÊNCIA DE PRESO</t>
-  </si>
-  <si>
-    <t>Relator_ELLEN GRACIE</t>
-  </si>
-  <si>
-    <t>origem_BA - BAHIA</t>
-  </si>
-  <si>
-    <t>origem_ES - ESPÍRITO SANTO</t>
-  </si>
-  <si>
-    <t>origem_RJ - RIO DE JANEIRO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A FÉ PÚBLICA</t>
-  </si>
-  <si>
-    <t>origem_GO - GOIÁS</t>
-  </si>
-  <si>
-    <t>assuntos ABOLITIO CRIMINIS</t>
-  </si>
-  <si>
-    <t>assuntos EFEITOS DA CONDENAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>origem_MT - MATO GROSSO</t>
-  </si>
-  <si>
-    <t>origem_PR - PARANÁ</t>
-  </si>
-  <si>
-    <t>assuntos ATO / NEGÓCIO JURÍDICO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A LIBERDADE PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos PENA RESTRITIVA DE DIREITOS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR PARTICULAR CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO (ART. 157)</t>
-  </si>
-  <si>
-    <t>assuntos MEDIDAS SÓCIO-EDUCATIVAS</t>
-  </si>
-  <si>
-    <t>assuntos RECEPTAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos GARANTIAS CONSTITUCIONAIS</t>
-  </si>
-  <si>
-    <t>assuntos DESPENALIZAÇÃO / DESCRIMINALIZAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A ORDEM TRIBUTÁRIA</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos ELEIÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos HOMICÍDIO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos FURTO</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DO MP</t>
-  </si>
-  <si>
-    <t>assuntos EXTINÇÃO DA PUNIBILIDADE</t>
-  </si>
-  <si>
-    <t>assuntos FURTO QUALIFICADO</t>
-  </si>
-  <si>
-    <t>assuntos AÇÃO PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS - LIBERATÓRIO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos VIOLÊNCIA DOMÉSTICA CONTRA A MULHER</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>assuntos AFASTAMENTO DO CARGO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES ELEITORAIS</t>
-  </si>
-  <si>
-    <t>assuntos PERDA DA FUNÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos CORRUPÇÃO PASSIVA</t>
-  </si>
-  <si>
-    <t>assuntos EXTRADIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PRATICADOS POR FUNCIONÁRIOS PÚBLICOS CONTRA A ADMINISTRAÇÃO EM GERAL</t>
-  </si>
-  <si>
-    <t>assuntos DE TRÁFICO ILÍCITO E USO INDEVIDO DE DROGAS</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES PREVISTOS NA LEI DA ORGANIZAÇÃO CRIMINOSA</t>
-  </si>
-  <si>
-    <t>assuntos APROPRIAÇÃO INDÉBITA</t>
-  </si>
-  <si>
-    <t>assuntos PARTE GERAL</t>
-  </si>
-  <si>
-    <t>assuntos ENTIDADES ADMINISTRATIVAS / ADMINISTRAÇÃO PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA MILITAR DA UNIÃO</t>
-  </si>
-  <si>
-    <t>assuntos SUSPENSÃO CONDICIONAL DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos NULIDADE OU ANULAÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos INDEFERIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos AGENTES POLÍTICOS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PENAL</t>
-  </si>
-  <si>
-    <t>assuntos TIPICIDADE</t>
-  </si>
-  <si>
-    <t>assuntos SUSPEIÇÃO</t>
-  </si>
-  <si>
-    <t>assuntos FURTO (ART. 155)</t>
-  </si>
-  <si>
-    <t>assuntos Desconhecido</t>
-  </si>
-  <si>
-    <t>assuntos ROUBO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ELEITORAL</t>
-  </si>
-  <si>
-    <t>assuntos CONTRABANDO OU DESCAMINHO</t>
-  </si>
-  <si>
-    <t>assuntos TRIBUNAL DE CONTAS</t>
-  </si>
-  <si>
-    <t>assuntos EXECUÇÃO PENAL PROVISÓRIA - CABIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos ASSOCIAÇÃO PARA A PRODUÇÃO E TRÁFICO E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>assuntos PREFEITO</t>
-  </si>
-  <si>
-    <t>assuntos FALSIFICAÇÃO DE DOCUMENTO PÚBLICO</t>
-  </si>
-  <si>
-    <t>assuntos TRÁFICO DE DROGAS E CONDUTAS AFINS</t>
-  </si>
-  <si>
-    <t>assuntos TRANCAMENTO - FALTA DE JUSTA CAUSA - COMPETÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos EMPRESAS</t>
-  </si>
-  <si>
-    <t>assuntos IMPEDIMENTO</t>
-  </si>
-  <si>
-    <t>assuntos COMPETÊNCIA DA JUSTIÇA ESTADUAL</t>
-  </si>
-  <si>
-    <t>assuntos POSSE DE DROGAS PARA CONSUMO PESSOAL</t>
-  </si>
-  <si>
-    <t>assuntos ESTELIONATO MAJORADO</t>
-  </si>
-  <si>
-    <t>assuntos ASSUNTOS DIVERSOS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO PROCESSUAL PENAL</t>
-  </si>
-  <si>
-    <t>assuntos TRANCAMENTO</t>
-  </si>
-  <si>
-    <t>assuntos APLICAÇÃO DA PENA</t>
-  </si>
-  <si>
-    <t>assuntos ATO INFRACIONAL</t>
-  </si>
-  <si>
-    <t>assuntos INTERNAÇÃO SEM ATIVIDADES EXTERNAS</t>
-  </si>
-  <si>
-    <t>assuntos CONTRA A VIDA</t>
-  </si>
-  <si>
-    <t>assuntos PREVISTOS NA LEGISLAÇÃO EXTRAVAGANTE</t>
-  </si>
-  <si>
-    <t>assuntos INSERÇÃO DE DADOS FALSOS EM SISTEMA DE INFORMAÇÕES</t>
-  </si>
-  <si>
-    <t>assuntos RECEPTAÇÃO QUALIFICADA</t>
-  </si>
-  <si>
-    <t>assuntos RECUPERAÇÃO JUDICIAL E FALÊNCIA</t>
-  </si>
-  <si>
-    <t>assuntos HABEAS CORPUS</t>
-  </si>
-  <si>
-    <t>assuntos DIREITO ELEITORAL E PROCESSO ELEITORAL</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES CONTRA A PAZ PÚBLICA</t>
-  </si>
-  <si>
-    <t>assuntos CRIMES MILITARES</t>
-  </si>
-  <si>
-    <t>assuntos FATOS JURÍDICOS</t>
   </si>
   <si>
     <t>assuntos FURTO DE COISA COMUM</t>
@@ -1002,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.45703125</v>
+        <v>0.3267024937247063</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.05859375</v>
+        <v>0.05559342843810917</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.03125</v>
+        <v>0.02404050487505688</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.01953125</v>
+        <v>0.02247358167289231</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.01171875</v>
+        <v>0.02206520426508173</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.0078125</v>
+        <v>0.0198338219996068</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.0078125</v>
+        <v>0.01718953371894287</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.0078125</v>
+        <v>0.01536616076392898</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.0078125</v>
+        <v>0.01531049796267871</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.0078125</v>
+        <v>0.01383480576709843</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.0078125</v>
+        <v>0.01375090959562491</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.0078125</v>
+        <v>0.013662045897221</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.0078125</v>
+        <v>0.01360772204590655</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.0078125</v>
+        <v>0.0120464055491339</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.0078125</v>
+        <v>0.01201524730101156</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.0078125</v>
+        <v>0.01190717008724762</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.0078125</v>
+        <v>0.01175775816371404</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.0078125</v>
+        <v>0.01143606353897668</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.0078125</v>
+        <v>0.01130550555480283</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.00390625</v>
+        <v>0.01023971012150689</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.00390625</v>
+        <v>0.01001754944611098</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1170,7 +1170,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.00390625</v>
+        <v>0.00972921198750409</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.00390625</v>
+        <v>0.0096081605927529</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.00390625</v>
+        <v>0.009135007537092777</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.00390625</v>
+        <v>0.009040233325970478</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.00390625</v>
+        <v>0.009013464283733988</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1210,7 +1210,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.00390625</v>
+        <v>0.008555982276746282</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1218,7 +1218,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.00390625</v>
+        <v>0.007852535271007415</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>0.00390625</v>
+        <v>0.007599755745630106</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.00390625</v>
+        <v>0.007485412177708949</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0.00390625</v>
+        <v>0.007271457671505485</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0.00390625</v>
+        <v>0.007241680316515864</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0.00390625</v>
+        <v>0.006886711317920531</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1266,7 +1266,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0.00390625</v>
+        <v>0.006741782921926768</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0.00390625</v>
+        <v>0.006595121839875609</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0.00390625</v>
+        <v>0.006577827269374815</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0.00390625</v>
+        <v>0.006499803566821205</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1298,7 +1298,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0.00390625</v>
+        <v>0.006454667546709744</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0.00390625</v>
+        <v>0.006445430997456928</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0.00390625</v>
+        <v>0.006141584531943296</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.00390625</v>
+        <v>0.005856735214301814</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0.00390625</v>
+        <v>0.005678190005674114</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.00390625</v>
+        <v>0.005566912319314943</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>0.00390625</v>
+        <v>0.005403953272440808</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>0.00390625</v>
+        <v>0.005392857664714949</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0.00390625</v>
+        <v>0.005308596108002429</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0.00390625</v>
+        <v>0.005271230714755527</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0.00390625</v>
+        <v>0.005172434817322638</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0.00390625</v>
+        <v>0.005083103778514176</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.00390625</v>
+        <v>0.005060303676082378</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0.00390625</v>
+        <v>0.005057284099462506</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0.00390625</v>
+        <v>0.00502723601445813</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0.00390625</v>
+        <v>0.004954655274818777</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0.00390625</v>
+        <v>0.004759671854737074</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0.00390625</v>
+        <v>0.004258017065967701</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.00390625</v>
+        <v>0.004059594409401544</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>0.00390625</v>
+        <v>0.003674383061898826</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0.00390625</v>
+        <v>0.003674052993305621</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0.00390625</v>
+        <v>0.003348962740450067</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0.00390625</v>
+        <v>0.003314941935655106</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0.00390625</v>
+        <v>0.003233160475955524</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0.00390625</v>
+        <v>0.003123257646696139</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>0.00390625</v>
+        <v>0.002702054728634887</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0.00390625</v>
+        <v>0.002512485048350286</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>0.00390625</v>
+        <v>0.002439530949144626</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>0.00390625</v>
+        <v>0.002229885076867081</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1530,7 +1530,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>0.00390625</v>
+        <v>0.002132862600033603</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1538,7 +1538,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>0.00390625</v>
+        <v>0.002062319052752457</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1546,7 +1546,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>0.00390625</v>
+        <v>0.002048963018209182</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1554,7 +1554,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>0.00390625</v>
+        <v>0.00204823882005979</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1562,7 +1562,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>0.00390625</v>
+        <v>0.002029376253352285</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1570,7 +1570,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>0.00390625</v>
+        <v>0.002011626906830119</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1578,7 +1578,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>0.00390625</v>
+        <v>0.002002908265224402</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1586,7 +1586,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>0.00390625</v>
+        <v>0.001995236963822517</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1594,7 +1594,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>0.00390625</v>
+        <v>0.001994068508926721</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1602,7 +1602,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>0.00390625</v>
+        <v>0.001984560632772427</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1610,7 +1610,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>0.00390625</v>
+        <v>0.001977832941638754</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1618,7 +1618,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>0.00390625</v>
+        <v>0.001974819861798261</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1626,7 +1626,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>0.00390625</v>
+        <v>0.001969298195362384</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1634,7 +1634,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>0.00390625</v>
+        <v>0.001968194319337372</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1642,7 +1642,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>0.00390625</v>
+        <v>0.00196036532477535</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1650,7 +1650,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>0.00390625</v>
+        <v>0.001959933723558053</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1658,7 +1658,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>0.00390625</v>
+        <v>0.001958997957157087</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1666,7 +1666,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>0.00390625</v>
+        <v>0.001951009329621973</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1674,7 +1674,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>0.00390625</v>
+        <v>0.001948729210127967</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>0.00390625</v>
+        <v>0.00194869668094312</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>0.00390625</v>
+        <v>0.001946316276441947</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1698,7 +1698,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>0.00390625</v>
+        <v>0.001936951804637616</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1706,7 +1706,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>0.00390625</v>
+        <v>0.001915320457637684</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1714,7 +1714,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>0.00390625</v>
+        <v>0.001903341734775598</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>0.00390625</v>
+        <v>0.001902623799643478</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1730,7 +1730,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>0.00390625</v>
+        <v>0.001874428793054555</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1738,7 +1738,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>0.00390625</v>
+        <v>0.001857286981790818</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1746,7 +1746,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>0.00390625</v>
+        <v>0.001775807626057801</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1754,7 +1754,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>0.00390625</v>
+        <v>0.001679652492996738</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1762,7 +1762,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>0.00390625</v>
+        <v>0.001676364923132918</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1770,7 +1770,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>0.00390625</v>
+        <v>0.001670066776748034</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1778,7 +1778,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>0.00390625</v>
+        <v>0.001624500502851752</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1786,7 +1786,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>0.00390625</v>
+        <v>0.001620940712613843</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1794,7 +1794,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>0.001484647226424172</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1802,7 +1802,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>0.001352332014492533</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1810,7 +1810,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>0.001331998862455351</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1818,7 +1818,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>0.00132833559084252</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1826,7 +1826,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>0.001284572726529577</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1834,7 +1834,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>0.001200403781595905</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1842,7 +1842,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>0.001149984263200798</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1850,7 +1850,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>0.001099069952635925</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1858,7 +1858,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>0.001049796979057642</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1866,7 +1866,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>0.0009724836363195449</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1874,7 +1874,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>0.0009566743749833917</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1882,7 +1882,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>0.0009210773847091141</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1890,7 +1890,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>0.00088781854953438</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1898,7 +1898,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>0.0004266571853410502</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1906,7 +1906,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>4.484425939810925E-05</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1914,7 +1914,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>2.219149309289683E-06</v>
       </c>
     </row>
     <row r="117" spans="1:2">

</xml_diff>